<commit_message>
update the IWB-JPI, add time-series model
</commit_message>
<xml_diff>
--- a/data/redclay_D47.xlsx
+++ b/data/redclay_D47.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiawei/Documents/Work/2023- redclay aridity/RedClay_jet/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiawei/Documents/Work/2023- redclay westerly/RedClay_jet/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F1C12C-587E-F74D-8C6F-D1A5DC641523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0650567-BBEF-7E4E-882C-7EC8B90769D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1260" windowWidth="25800" windowHeight="16540" xr2:uid="{E59976B8-B089-8E41-A9BF-C50A2DC09617}"/>
+    <workbookView xWindow="13200" yWindow="2240" windowWidth="25800" windowHeight="16540" xr2:uid="{E59976B8-B089-8E41-A9BF-C50A2DC09617}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$J$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$L$33</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>SL10</t>
   </si>
@@ -120,15 +120,18 @@
   </si>
   <si>
     <t>Jiaxian</t>
+  </si>
+  <si>
+    <t>D47</t>
+  </si>
+  <si>
+    <t>D47.se</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -166,10 +169,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,18 +509,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA88B5D3-B159-6A44-B862-C9AB8CA5CD5F}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="9" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="12" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -541,14 +547,20 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -573,14 +585,20 @@
       <c r="H2" s="1">
         <v>6.4716857669904482E-2</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
+        <v>0.60937000000000008</v>
+      </c>
+      <c r="J2" s="3">
+        <v>9.9107808355766453E-3</v>
+      </c>
+      <c r="K2" s="2">
         <v>19.876009535897936</v>
       </c>
-      <c r="J2" s="2">
+      <c r="L2" s="2">
         <v>3.2417566367586232</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -605,14 +623,20 @@
       <c r="H3" s="1">
         <v>4.4948933246518559E-2</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
+        <v>0.61250599999999999</v>
+      </c>
+      <c r="J3" s="3">
+        <v>8.7434939240557466E-3</v>
+      </c>
+      <c r="K3" s="2">
         <v>18.872199071806733</v>
       </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2">
         <v>2.8644912336736184</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -626,25 +650,31 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>-1.7302199999999999</v>
+        <v>-2.0855750000000004</v>
       </c>
       <c r="F4" s="1">
-        <v>4.120603111196218E-2</v>
+        <v>5.0007357791962366E-2</v>
       </c>
       <c r="G4" s="1">
-        <v>-9.7329600000000003</v>
+        <v>-9.6923999999999992</v>
       </c>
       <c r="H4" s="1">
-        <v>4.7947674604718812E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>23.808274939364026</v>
-      </c>
-      <c r="J4" s="2">
-        <v>3.3755433336655756</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5.7485345958774539E-2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.61161999999999994</v>
+      </c>
+      <c r="J4" s="3">
+        <v>9.9107808355766453E-3</v>
+      </c>
+      <c r="K4" s="2">
+        <v>19.154755075255196</v>
+      </c>
+      <c r="L4" s="2">
+        <v>3.2176142270322998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -658,25 +688,31 @@
         <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>-2.0855750000000004</v>
+        <v>-1.7302199999999999</v>
       </c>
       <c r="F5" s="1">
-        <v>5.0007357791962366E-2</v>
+        <v>4.120603111196218E-2</v>
       </c>
       <c r="G5" s="1">
-        <v>-9.6923999999999992</v>
+        <v>-9.7329600000000003</v>
       </c>
       <c r="H5" s="1">
-        <v>5.7485345958774539E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>19.154755075255196</v>
-      </c>
-      <c r="J5" s="2">
-        <v>3.2176142270322998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4.7947674604718812E-2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.59739000000000009</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9.9107808355766453E-3</v>
+      </c>
+      <c r="K5" s="2">
+        <v>23.808274939364026</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3.3755433336655756</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -701,14 +737,20 @@
       <c r="H6" s="1">
         <v>4.4254348938833003E-2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
+        <v>0.58465000000000011</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.2864520200924722E-2</v>
+      </c>
+      <c r="K6" s="2">
         <v>28.168747084730001</v>
       </c>
-      <c r="J6" s="2">
+      <c r="L6" s="2">
         <v>4.603955831740393</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -733,14 +775,20 @@
       <c r="H7" s="1">
         <v>8.3171132562125605E-2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
+        <v>0.61113249999999997</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.1018905250371585E-2</v>
+      </c>
+      <c r="K7" s="2">
         <v>19.310574883671279</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>3.5898234017836899</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -765,14 +813,20 @@
       <c r="H8" s="1">
         <v>9.2394089517553873E-2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
+        <v>0.60386666666666666</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K8" s="2">
         <v>21.66289214554763</v>
       </c>
-      <c r="J8" s="2">
+      <c r="L8" s="2">
         <v>3.8229092612070872</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -797,14 +851,20 @@
       <c r="H9" s="1">
         <v>5.3057184244925559E-2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
+        <v>0.61226599999999998</v>
+      </c>
+      <c r="J9" s="3">
+        <v>8.8644718633806175E-3</v>
+      </c>
+      <c r="K9" s="2">
         <v>18.948657017655535</v>
       </c>
-      <c r="J9" s="2">
+      <c r="L9" s="2">
         <v>2.8667639494097443</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -829,14 +889,20 @@
       <c r="H10" s="1">
         <v>6.8714911045565708E-2</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
+        <v>0.58727800000000008</v>
+      </c>
+      <c r="J10" s="3">
+        <v>8.8644718633806175E-3</v>
+      </c>
+      <c r="K10" s="2">
         <v>27.253549375414536</v>
       </c>
-      <c r="J10" s="2">
+      <c r="L10" s="2">
         <v>3.120962549604883</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -861,14 +927,20 @@
       <c r="H11" s="1">
         <v>2.1853019115089332E-2</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
+        <v>0.60670333333333337</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K11" s="2">
         <v>20.737782898971716</v>
       </c>
-      <c r="J11" s="2">
+      <c r="L11" s="2">
         <v>3.7865702378138053</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -893,14 +965,20 @@
       <c r="H12" s="1">
         <v>3.718827473516071E-2</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
+        <v>0.62392666666666674</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K12" s="2">
         <v>15.301853208963337</v>
       </c>
-      <c r="J12" s="2">
+      <c r="L12" s="2">
         <v>3.577771533307498</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -925,14 +1003,20 @@
       <c r="H13" s="1">
         <v>9.0551379890093264E-2</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
+        <v>0.62030600000000002</v>
+      </c>
+      <c r="J13" s="3">
+        <v>8.8644718633806175E-3</v>
+      </c>
+      <c r="K13" s="2">
         <v>16.419540452839669</v>
       </c>
-      <c r="J13" s="2">
+      <c r="L13" s="2">
         <v>2.7922307476620176</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -957,14 +1041,20 @@
       <c r="H14" s="1">
         <v>5.7166423711825891E-3</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="3">
+        <v>0.62319333333333338</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K14" s="2">
         <v>15.527185448826003</v>
       </c>
-      <c r="J14" s="2">
+      <c r="L14" s="2">
         <v>3.5862674307954308</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -989,14 +1079,20 @@
       <c r="H15" s="1">
         <v>1.9317033358613029E-2</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="3">
+        <v>0.60861999999999994</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K15" s="2">
         <v>20.117616748277499</v>
       </c>
-      <c r="J15" s="2">
+      <c r="L15" s="2">
         <v>3.7623414937407347</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1021,14 +1117,20 @@
       <c r="H16" s="1">
         <v>0.1166971436382801</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="3">
+        <v>0.61276666666666679</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K16" s="2">
         <v>18.789225226330586</v>
       </c>
-      <c r="J16" s="2">
+      <c r="L16" s="2">
         <v>3.7107985745471979</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1053,14 +1155,20 @@
       <c r="H17" s="1">
         <v>1.3451187473396006E-2</v>
       </c>
-      <c r="I17" s="2">
-        <v>11.520667820973401</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="I17" s="3">
+        <v>0.63649333333333336</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>11.520667820973358</v>
+      </c>
+      <c r="L17" s="2">
         <v>3.4372372503634097</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1085,14 +1193,20 @@
       <c r="H18" s="1">
         <v>6.9252519087755815E-2</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="3">
+        <v>0.60244800000000009</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.8623758857974942E-2</v>
+      </c>
+      <c r="K18" s="2">
         <v>22.128844684422916</v>
       </c>
-      <c r="J18" s="2">
+      <c r="L18" s="2">
         <v>6.3292034814500653</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1117,14 +1231,20 @@
       <c r="H19" s="1">
         <v>1.3131810402394924E-2</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="3">
+        <v>0.60686666666666667</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1.1443983966599122E-2</v>
+      </c>
+      <c r="K19" s="2">
         <v>20.684780543470254</v>
       </c>
-      <c r="J19" s="2">
+      <c r="L19" s="2">
         <v>3.7844954024072308</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1149,14 +1269,20 @@
       <c r="H20" s="1">
         <v>2.0449173852560041E-2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="3">
+        <v>0.63162277215675078</v>
+      </c>
+      <c r="J20" s="3">
+        <v>9.1036059432753787E-3</v>
+      </c>
+      <c r="K20" s="2">
         <v>12.968451685594914</v>
       </c>
-      <c r="J20" s="2">
+      <c r="L20" s="2">
         <v>2.76635249156692</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1181,14 +1307,20 @@
       <c r="H21" s="1">
         <v>8.8769421485821315E-2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="3">
+        <v>0.62268988791059277</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1.1143048194318274E-2</v>
+      </c>
+      <c r="K21" s="2">
         <v>15.682185807029896</v>
       </c>
-      <c r="J21" s="2">
+      <c r="L21" s="2">
         <v>3.4959376342322912</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1213,14 +1345,20 @@
       <c r="H22" s="1">
         <v>4.2248175636962648E-2</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="3">
+        <v>0.5970259694588943</v>
+      </c>
+      <c r="J22" s="3">
+        <v>1.1149594690196508E-2</v>
+      </c>
+      <c r="K22" s="2">
         <v>23.93025388810554</v>
       </c>
-      <c r="J22" s="2">
+      <c r="L22" s="2">
         <v>3.8103702005366245</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1245,14 +1383,20 @@
       <c r="H23" s="1">
         <v>6.0603583517646338E-2</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="3">
+        <v>0.58896553707536825</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1.3156516599989584E-2</v>
+      </c>
+      <c r="K23" s="2">
         <v>26.670244795805957</v>
       </c>
-      <c r="J23" s="2">
+      <c r="L23" s="2">
         <v>4.63989833207836</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1277,14 +1421,20 @@
       <c r="H24" s="1">
         <v>2.9788543295294099E-2</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="3">
+        <v>0.59374032935495669</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1.2874442991480353E-2</v>
+      </c>
+      <c r="K24" s="2">
         <v>25.038046617078123</v>
       </c>
-      <c r="J24" s="2">
+      <c r="L24" s="2">
         <v>4.4633304199505801</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1309,14 +1459,20 @@
       <c r="H25" s="1">
         <v>4.3600866457383161E-2</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="3">
+        <v>0.63394049675425823</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2.406488814384123E-2</v>
+      </c>
+      <c r="K25" s="2">
         <v>12.276755184830392</v>
       </c>
-      <c r="J25" s="2">
+      <c r="L25" s="2">
         <v>7.4367126693729233</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1341,14 +1497,20 @@
       <c r="H26" s="1">
         <v>3.3760186626402802E-2</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="3">
+        <v>0.6082575213625887</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1.2874442991480353E-2</v>
+      </c>
+      <c r="K26" s="2">
         <v>20.234601105366096</v>
       </c>
-      <c r="J26" s="2">
+      <c r="L26" s="2">
         <v>4.2480269012189069</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1373,14 +1535,20 @@
       <c r="H27" s="1">
         <v>1.6249043280388713E-2</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="3">
+        <v>0.60387054669681228</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1.1149594690196508E-2</v>
+      </c>
+      <c r="K27" s="2">
         <v>21.661620796063119</v>
       </c>
-      <c r="J27" s="2">
-        <v>3.7226479193466799</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L27" s="2">
+        <v>3.7226479193466844</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1405,14 +1573,20 @@
       <c r="H28" s="1">
         <v>4.5154620150258833E-2</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="3">
+        <v>0.6324698126760625</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1.5767908025838946E-2</v>
+      </c>
+      <c r="K28" s="2">
         <v>12.715080134248979</v>
       </c>
-      <c r="J28" s="2">
+      <c r="L28" s="2">
         <v>4.8300357890543069</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1437,14 +1611,20 @@
       <c r="H29" s="1">
         <v>4.5658756380161515E-2</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="3">
+        <v>0.61064588201145686</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1.1310350048962374E-2</v>
+      </c>
+      <c r="K29" s="2">
         <v>19.466361553471131</v>
       </c>
-      <c r="J29" s="2">
+      <c r="L29" s="2">
         <v>3.6925443715024926</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1469,14 +1649,20 @@
       <c r="H30" s="1">
         <v>6.7011657570791042E-2</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="3">
+        <v>0.57804183092840655</v>
+      </c>
+      <c r="J30" s="3">
+        <v>9.9725006595400394E-3</v>
+      </c>
+      <c r="K30" s="2">
         <v>30.50751118731722</v>
       </c>
-      <c r="J30" s="2">
+      <c r="L30" s="2">
         <v>3.6349081932336276</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1501,14 +1687,20 @@
       <c r="H31" s="1">
         <v>4.525969079669119E-2</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="3">
+        <v>0.60480120840361073</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9.9725006595400394E-3</v>
+      </c>
+      <c r="K31" s="2">
         <v>21.357149962857648</v>
       </c>
-      <c r="J31" s="2">
+      <c r="L31" s="2">
         <v>3.3125653887054796</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1533,14 +1725,20 @@
       <c r="H32" s="1">
         <v>3.9413764360303402E-2</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="3">
+        <v>0.6327616003982609</v>
+      </c>
+      <c r="J32" s="3">
+        <v>1.5454693393834229E-2</v>
+      </c>
+      <c r="K32" s="2">
         <v>12.627954690684078</v>
       </c>
-      <c r="J32" s="2">
+      <c r="L32" s="2">
         <v>4.727299308431725</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1565,16 +1763,22 @@
       <c r="H33" s="1">
         <v>6.964658924406758E-2</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="3">
+        <v>0.62509490679408686</v>
+      </c>
+      <c r="J33" s="3">
+        <v>9.9725006595400394E-3</v>
+      </c>
+      <c r="K33" s="2">
         <v>14.943973937602721</v>
       </c>
-      <c r="J33" s="2">
+      <c r="L33" s="2">
         <v>3.0985803905993521</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J33" xr:uid="{AA88B5D3-B159-6A44-B862-C9AB8CA5CD5F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J33">
+  <autoFilter ref="A1:L33" xr:uid="{AA88B5D3-B159-6A44-B862-C9AB8CA5CD5F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L33">
       <sortCondition ref="A1:A33"/>
     </sortState>
   </autoFilter>

</xml_diff>